<commit_message>
Changed the connection of posts with users, added a new dto to the post, the user returns with the post, added a synchronous request from SC to US
</commit_message>
<xml_diff>
--- a/socialservice/src/main/resources/DB.xlsx
+++ b/socialservice/src/main/resources/DB.xlsx
@@ -4,17 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="profile" sheetId="1" r:id="rId1"/>
+    <sheet name="post" sheetId="1" r:id="rId1"/>
+    <sheet name="friend_request" sheetId="2" r:id="rId2"/>
+    <sheet name="friendships" sheetId="3" r:id="rId3"/>
+    <sheet name="subscriptions" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>UUID</t>
   </si>
@@ -35,6 +38,33 @@
   </si>
   <si>
     <t>title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">status </t>
+  </si>
+  <si>
+    <t>user1_id</t>
+  </si>
+  <si>
+    <t>user2_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">follower_id </t>
+  </si>
+  <si>
+    <t>followed_user_id</t>
+  </si>
+  <si>
+    <t>Кто подписался</t>
+  </si>
+  <si>
+    <t>На кого подписался</t>
+  </si>
+  <si>
+    <t>sender_uuid</t>
+  </si>
+  <si>
+    <t>receiver_uuid</t>
   </si>
 </sst>
 </file>
@@ -378,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -419,4 +449,107 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="14.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="20.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>